<commit_message>
[Refactor] use drive path, modify knit output file, add imgs
</commit_message>
<xml_diff>
--- a/data/Client List.xlsx
+++ b/data/Client List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/warsameyusuf/Documents/Masters/Research project/Git files BLL/covid-19-wastewater/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D119AF-4276-434B-9A0B-239B158E4E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435FBD03-6191-D846-90EF-4D863A3EC8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25120" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>sample101@ottawa.ca</t>
+  </si>
+  <si>
+    <t>CSC</t>
   </si>
 </sst>
 </file>
@@ -414,7 +417,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -481,6 +484,9 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>